<commit_message>
update according to new partition table
</commit_message>
<xml_diff>
--- a/Documents/specs/ESP32_Memory_Map.xlsx
+++ b/Documents/specs/ESP32_Memory_Map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="10512" windowHeight="7956" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Single_NO_OTA" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="51">
   <si>
     <t>Memory
 ADDR</t>
@@ -181,6 +181,15 @@
       </rPr>
       <t>1K a cosa serve è per caso il certificato !!!!!!</t>
     </r>
+  </si>
+  <si>
+    <t>0x2000</t>
+  </si>
+  <si>
+    <t>0x190000</t>
+  </si>
+  <si>
+    <t>0x180000</t>
   </si>
 </sst>
 </file>
@@ -521,11 +530,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1049,7 +1058,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1374,10 +1383,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1503,7 +1512,7 @@
       <c r="A11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="77">
+      <c r="B11" s="76">
         <v>24576</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -1557,7 +1566,9 @@
       <c r="A16" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="67"/>
+      <c r="B16" s="67" t="s">
+        <v>48</v>
+      </c>
       <c r="C16" s="45" t="s">
         <v>20</v>
       </c>
@@ -1582,13 +1593,13 @@
       <c r="F18" s="43"/>
     </row>
     <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.3">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="76">
-        <v>4096</v>
-      </c>
-      <c r="C19" s="36" t="s">
+      <c r="B19" s="77" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="28" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="28" t="s">
@@ -1610,32 +1621,28 @@
       <c r="F20" s="31"/>
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="30"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
-      <c r="F21" s="31"/>
-    </row>
-    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="46" t="s">
+      <c r="F21" s="34"/>
+    </row>
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="A22" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="47" t="s">
-        <v>10</v>
+      <c r="B22" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="53" t="s">
+        <v>22</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="48" t="s">
-        <v>13</v>
-      </c>
+      <c r="E22" s="12"/>
+      <c r="F22" s="60"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="49"/>
@@ -1655,19 +1662,19 @@
     </row>
     <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.3">
       <c r="A25" s="52" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B25" s="53" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C25" s="53" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D25" s="69" t="s">
         <v>34</v>
       </c>
       <c r="E25" s="53" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F25" s="51"/>
     </row>
@@ -1679,63 +1686,29 @@
       <c r="E26" s="50"/>
       <c r="F26" s="51"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="57"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="59"/>
-    </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="69" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="51"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="49"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="51"/>
-    </row>
-    <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="54"/>
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="56"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="70" t="s">
+    <row r="27" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="54"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="56"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="70" t="s">
+      <c r="B28" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="70" t="s">
+      <c r="C28" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70" t="s">
+      <c r="D28" s="70"/>
+      <c r="E28" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="F31" s="70"/>
+      <c r="F28" s="70"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>